<commit_message>
extra analysis at Greater Melbourne level
</commit_message>
<xml_diff>
--- a/output/accessibility tables.xlsx
+++ b/output/accessibility tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\MEGAsync\Steve\RMIT JIBE\20mnMelbourne\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1C641-0AD7-4F28-A471-D01E78C6A92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED20D97C-3A4C-4C69-BECB-FF56A4D46CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17385" yWindow="-15855" windowWidth="24765" windowHeight="14310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="-15465" windowWidth="24720" windowHeight="13410" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LGA accessibility scores walk" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,27 @@
     <sheet name="LGA accessibility scores summ" sheetId="3" r:id="rId3"/>
     <sheet name="SA2 accessibility scores walk" sheetId="4" r:id="rId4"/>
     <sheet name="SA2 accessibility scores cycle" sheetId="5" r:id="rId5"/>
+    <sheet name="people &amp; dwelling access scores" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="434">
   <si>
     <t>NAME</t>
   </si>
@@ -1300,6 +1314,33 @@
   <si>
     <t>214021385</t>
   </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>walk_dwel_base</t>
+  </si>
+  <si>
+    <t>walk_dwel_int</t>
+  </si>
+  <si>
+    <t>walk_people_base</t>
+  </si>
+  <si>
+    <t>walk_people_int</t>
+  </si>
+  <si>
+    <t>cycle_dwel_base</t>
+  </si>
+  <si>
+    <t>cycle_dwel_int</t>
+  </si>
+  <si>
+    <t>cycle_people_base</t>
+  </si>
+  <si>
+    <t>cycle_people_int</t>
+  </si>
 </sst>
 </file>
 
@@ -1308,13 +1349,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -1345,11 +1391,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1653,26 +1700,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="5" width="10.90625" style="1"/>
-    <col min="6" max="6" width="10.90625" style="2"/>
-    <col min="7" max="7" width="10.90625" style="3"/>
-    <col min="8" max="9" width="10.90625" style="1"/>
-    <col min="10" max="10" width="10.90625" style="2"/>
-    <col min="11" max="11" width="10.90625" style="3"/>
-    <col min="12" max="13" width="10.90625" style="1"/>
-    <col min="14" max="14" width="10.90625" style="2"/>
-    <col min="15" max="15" width="10.90625" style="3"/>
-    <col min="16" max="17" width="10.90625" style="1"/>
-    <col min="18" max="18" width="10.90625" style="2"/>
-    <col min="19" max="19" width="10.90625" style="3"/>
-    <col min="20" max="21" width="10.90625" style="1"/>
-    <col min="22" max="22" width="10.90625" style="2"/>
-    <col min="23" max="23" width="10.90625" style="3"/>
-    <col min="24" max="25" width="10.90625" style="1"/>
-    <col min="26" max="26" width="10.90625" style="2"/>
-    <col min="27" max="27" width="10.90625" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -4333,8 +4360,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Calibri"</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -4343,31 +4370,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="5" width="10.90625" style="1"/>
-    <col min="6" max="6" width="10.90625" style="2"/>
-    <col min="7" max="7" width="10.90625" style="3"/>
-    <col min="8" max="9" width="10.90625" style="1"/>
-    <col min="10" max="10" width="10.90625" style="2"/>
-    <col min="11" max="11" width="10.90625" style="3"/>
-    <col min="12" max="13" width="10.90625" style="1"/>
-    <col min="14" max="14" width="10.90625" style="2"/>
-    <col min="15" max="15" width="10.90625" style="3"/>
-    <col min="16" max="17" width="10.90625" style="1"/>
-    <col min="18" max="18" width="10.90625" style="2"/>
-    <col min="19" max="19" width="10.90625" style="3"/>
-    <col min="20" max="21" width="10.90625" style="1"/>
-    <col min="22" max="22" width="10.90625" style="2"/>
-    <col min="23" max="23" width="10.90625" style="3"/>
-    <col min="24" max="25" width="10.90625" style="1"/>
-    <col min="26" max="26" width="10.90625" style="2"/>
-    <col min="27" max="27" width="10.90625" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -7028,8 +7035,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Calibri"</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -7043,14 +7050,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="4" width="10.90625" style="1"/>
-    <col min="5" max="5" width="10.90625" style="2"/>
-    <col min="6" max="6" width="10.90625" style="3"/>
-    <col min="7" max="8" width="10.90625" style="1"/>
-    <col min="9" max="9" width="10.90625" style="2"/>
-    <col min="10" max="10" width="10.90625" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -8079,8 +8078,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Calibri"</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -27271,8 +27270,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Calibri"</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -46463,8 +46462,491 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KEEDC00 RMIT Classification: Trusted&amp;1#_x000D_</oddHeader>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Calibri"</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="9" width="10.90625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4.0319528506803</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3.7741136959614501</v>
+      </c>
+      <c r="D2" s="4">
+        <v>4.2230671600012899</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3.9731616948168802</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.80555264028970996</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.79067411713075397</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.83924613253894698</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.82754750807152599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8.1908431929516006</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7.0520809788155301</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8.82069123082867</v>
+      </c>
+      <c r="E3" s="4">
+        <v>7.6462018850118598</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1.2952319495860101</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1.2307053139020101</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.2866926126217499</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.2266977144353699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8.3876135635347797</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6.26296347690195</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9.2165188535065408</v>
+      </c>
+      <c r="E4" s="4">
+        <v>7.0114166413995598</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.98212372471676301</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.83255460293532002</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.929911809400915</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.80706724602018398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8.9163134221016005</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5.5463565936763404</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.6166093053976809</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.1562039874765304</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.1918694602512001</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.92670302352259304</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.2109590973705899</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.967966107241374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9.7965604024877706</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.1266467454856004</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10.639846708916901</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.7799387123700301</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.0880185076132201</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.75676703971815396</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.1660942993402099</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.83897954924087403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>9.9483235253638593</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4.3176406255884698</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10.503008871478301</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4.7832787269863504</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1.30789459125748</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.78066316770827504</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.4631199601496201</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.88548283002111305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>9.2780000058252892</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.4529463675756702</v>
+      </c>
+      <c r="D8" s="4">
+        <v>9.5674931873834392</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3.7430007891078301</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.5569246975365301</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.86847988081772798</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.77704542804758</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.0139958438218699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8.4212445793023907</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.3817269099420701</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8.4824534487967398</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.5506427195042201</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.9563862907846401</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.80273653897029995</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2.0850567124563102</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.911795944821574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7.4338507589840201</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.0477325475825698</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7.1551158482136001</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2.1112582433063198</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2.63925354292346</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.77606366061855903</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3.0102713255018201</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.92240477450095004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6.9616499198240698</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.3636557383682502</v>
+      </c>
+      <c r="D11" s="4">
+        <v>6.4634570136142697</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.3749507806174601</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.9261272754661198</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.83288113806375397</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4.4783072614930903</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.978632951207422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6.7925903312180704</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3.39274907588426</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5.8888916949752899</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.4181674640547501</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.1844059730427796</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.89495088680403501</v>
+      </c>
+      <c r="H12" s="4">
+        <v>6.9862383562634296</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1.0165954799903401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>5.2376739541745101</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5.6386843101365498</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4.3107797114316799</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5.6514086308836404</v>
+      </c>
+      <c r="F13" s="4">
+        <v>9.6057422711559308</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.64014929453534</v>
+      </c>
+      <c r="H13" s="4">
+        <v>10.569184479630101</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1.8230786303062301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3.86010080313297</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8.5444691395260097</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3.06301657326201</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8.2850655146727608</v>
+      </c>
+      <c r="F14" s="4">
+        <v>15.224895292469</v>
+      </c>
+      <c r="G14" s="4">
+        <v>6.9657223196558098</v>
+      </c>
+      <c r="H14" s="4">
+        <v>15.8769360157211</v>
+      </c>
+      <c r="I14" s="4">
+        <v>7.7696150703847602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.2821168151946001</v>
+      </c>
+      <c r="C15" s="4">
+        <v>10.8387158390622</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.6716700020150399</v>
+      </c>
+      <c r="E15" s="4">
+        <v>9.7385830421202702</v>
+      </c>
+      <c r="F15" s="4">
+        <v>24.975707321192999</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5.2384385408243501</v>
+      </c>
+      <c r="H15" s="4">
+        <v>24.177883548450101</v>
+      </c>
+      <c r="I15" s="4">
+        <v>5.5192357883205796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.46116587522415697</v>
+      </c>
+      <c r="C16" s="4">
+        <v>29.259517955493099</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.37738039017858099</v>
+      </c>
+      <c r="E16" s="4">
+        <v>26.7767211676715</v>
+      </c>
+      <c r="F16" s="4">
+        <v>27.2598664617142</v>
+      </c>
+      <c r="G16" s="4">
+        <v>76.662510474792995</v>
+      </c>
+      <c r="H16" s="4">
+        <v>24.143052961014401</v>
+      </c>
+      <c r="I16" s="4">
+        <v>74.490904561615807</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>